<commit_message>
bugs and improvement sheet added
</commit_message>
<xml_diff>
--- a/Bugs_and_improvements.xlsx
+++ b/Bugs_and_improvements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KIIT\IdeaProjects\Myntra_Project_Final\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3FF60B98-F0BF-4F34-9708-7010CE1E5A44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48F0D109-BF06-42FE-8952-3E7836C3F99D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
   <si>
     <t>Category</t>
   </si>
@@ -83,20 +83,38 @@
 3. The side panel doesn't scroll to the bottom</t>
   </si>
   <si>
-    <t>SS</t>
-  </si>
-  <si>
-    <t>V</t>
+    <t>https://drive.google.com/file/d/12otaMISfL_ZA1ZJZAfrgk_m7H2egPVGe/view?usp=drive_link</t>
+  </si>
+  <si>
+    <t>1. Go to any category or section
+2. Some products have Discount price while there's discount percentage in others</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1CqYrWFFT0XQ8tdBdk14XpzIEf1l7xKaf/view?usp=drive_link</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1szzErH2C_SeYx8dBQnBm17Fh6eUC4X-V/view?usp=drive_link</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/file/d/1QleOHP9UNqrotyynYyLmnJcccMPow_R7/view?usp=drive_link</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -119,10 +137,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -139,8 +158,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -478,22 +502,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.5" customWidth="1"/>
     <col min="2" max="2" width="51.625" customWidth="1"/>
     <col min="3" max="3" width="112.25" customWidth="1"/>
     <col min="4" max="4" width="36.75" customWidth="1"/>
-    <col min="5" max="5" width="16.25" customWidth="1"/>
+    <col min="5" max="5" width="29.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -523,11 +547,11 @@
       <c r="D2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>18</v>
+      <c r="E2" s="7" t="s">
+        <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -537,8 +561,11 @@
       <c r="C3" t="s">
         <v>10</v>
       </c>
-      <c r="E3" t="s">
-        <v>18</v>
+      <c r="D3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -554,8 +581,8 @@
       <c r="D4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E4" t="s">
-        <v>19</v>
+      <c r="E4" s="6" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="63" x14ac:dyDescent="0.25">
@@ -571,13 +598,17 @@
       <c r="D5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="7" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25"/>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E5" r:id="rId1" xr:uid="{EA89A300-A3AF-4061-A93F-55CEF2AB7B40}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{74DD2817-1F60-4D0F-A2A0-9C696584FC03}"/>
+    <hyperlink ref="E2" r:id="rId3" xr:uid="{573BF383-CE07-43B6-9D1F-5949BDBBDB10}"/>
+    <hyperlink ref="E4" r:id="rId4" xr:uid="{D78343A4-7FEA-44B6-965E-954D7913C78C}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
     <ignoredError sqref="A1:C1 C2 A3 A4 A5" numberStoredAsText="1"/>

</xml_diff>